<commit_message>
ft: new champs && invoke params
</commit_message>
<xml_diff>
--- a/data/campeonato_10_1.xlsx
+++ b/data/campeonato_10_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="55">
   <si>
     <t>EQUIPO</t>
   </si>
@@ -80,82 +80,106 @@
     <t>3:0</t>
   </si>
   <si>
+    <t>3:4</t>
+  </si>
+  <si>
+    <t>3:3</t>
+  </si>
+  <si>
+    <t>6:0</t>
+  </si>
+  <si>
+    <t>2:5</t>
+  </si>
+  <si>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>3:2</t>
+  </si>
+  <si>
     <t>4:2</t>
   </si>
   <si>
+    <t>4:0</t>
+  </si>
+  <si>
+    <t>1:2</t>
+  </si>
+  <si>
+    <t>5:4</t>
+  </si>
+  <si>
     <t>0:2</t>
   </si>
   <si>
     <t>5:0</t>
   </si>
   <si>
+    <t>2:4</t>
+  </si>
+  <si>
+    <t>1:5</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>6:2</t>
+  </si>
+  <si>
+    <t>7:3</t>
+  </si>
+  <si>
+    <t>4:3</t>
+  </si>
+  <si>
+    <t>2:2</t>
+  </si>
+  <si>
+    <t>1:4</t>
+  </si>
+  <si>
+    <t>1:3</t>
+  </si>
+  <si>
+    <t>7:1</t>
+  </si>
+  <si>
+    <t>1:6</t>
+  </si>
+  <si>
+    <t>6:4</t>
+  </si>
+  <si>
+    <t>3:5</t>
+  </si>
+  <si>
     <t>3:1</t>
   </si>
   <si>
+    <t>1:0</t>
+  </si>
+  <si>
     <t>2:1</t>
   </si>
   <si>
-    <t>0:5</t>
-  </si>
-  <si>
-    <t>0:0</t>
+    <t>5:5</t>
+  </si>
+  <si>
+    <t>6:3</t>
+  </si>
+  <si>
+    <t>5:2</t>
   </si>
   <si>
     <t>0:4</t>
   </si>
   <si>
-    <t>3:4</t>
-  </si>
-  <si>
-    <t>3:2</t>
-  </si>
-  <si>
-    <t>2:0</t>
-  </si>
-  <si>
-    <t>1:0</t>
-  </si>
-  <si>
-    <t>2:3</t>
-  </si>
-  <si>
-    <t>5:1</t>
-  </si>
-  <si>
-    <t>0:1</t>
-  </si>
-  <si>
-    <t>0:3</t>
-  </si>
-  <si>
-    <t>1:1</t>
-  </si>
-  <si>
-    <t>3:3</t>
-  </si>
-  <si>
-    <t>1:2</t>
-  </si>
-  <si>
-    <t>2:2</t>
-  </si>
-  <si>
-    <t>1:5</t>
-  </si>
-  <si>
-    <t>4:5</t>
-  </si>
-  <si>
-    <t>4:0</t>
-  </si>
-  <si>
-    <t>2:4</t>
-  </si>
-  <si>
-    <t>1:3</t>
-  </si>
-  <si>
-    <t>5:2</t>
+    <t>4:1</t>
+  </si>
+  <si>
+    <t>3:6</t>
   </si>
 </sst>
 </file>
@@ -518,10 +542,10 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -535,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -552,10 +576,10 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -569,10 +593,10 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -586,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -603,10 +627,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -620,10 +644,10 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -637,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -654,10 +678,10 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -671,10 +695,10 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +708,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -709,7 +733,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -717,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -731,7 +755,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -745,10 +769,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -759,7 +783,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -776,15 +800,15 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -792,13 +816,13 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -806,13 +830,13 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -820,13 +844,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -840,7 +864,7 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -848,18 +872,18 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -867,13 +891,13 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -881,10 +905,10 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -895,13 +919,13 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -909,13 +933,13 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -923,18 +947,18 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -942,13 +966,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -956,13 +980,13 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -973,10 +997,10 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -984,13 +1008,13 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -998,18 +1022,18 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1017,13 +1041,13 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1031,13 +1055,13 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1045,10 +1069,10 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
         <v>36</v>
@@ -1059,13 +1083,13 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1073,18 +1097,18 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1092,13 +1116,13 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1109,10 +1133,10 @@
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1120,13 +1144,13 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1134,13 +1158,13 @@
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1148,18 +1172,18 @@
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1167,13 +1191,13 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1181,10 +1205,10 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E40" t="s">
         <v>27</v>
@@ -1195,13 +1219,13 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1209,13 +1233,13 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1223,18 +1247,18 @@
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1242,13 +1266,13 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1256,13 +1280,13 @@
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1270,13 +1294,13 @@
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E47" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1284,13 +1308,13 @@
         <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1298,18 +1322,18 @@
         <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1317,13 +1341,13 @@
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1331,13 +1355,13 @@
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1345,13 +1369,13 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1359,13 +1383,13 @@
         <v>19</v>
       </c>
       <c r="C54" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
         <v>12</v>
       </c>
-      <c r="D54" t="s">
-        <v>8</v>
-      </c>
       <c r="E54" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1373,18 +1397,18 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E55" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1392,13 +1416,13 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1406,13 +1430,13 @@
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E58" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1420,13 +1444,13 @@
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E59" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1434,13 +1458,13 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1448,18 +1472,18 @@
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1467,13 +1491,13 @@
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1481,13 +1505,13 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
         <v>13</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1495,13 +1519,13 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1509,13 +1533,13 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1523,18 +1547,18 @@
         <v>19</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1542,13 +1566,13 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E69" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1556,13 +1580,13 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1573,10 +1597,10 @@
         <v>8</v>
       </c>
       <c r="D71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1584,13 +1608,13 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D72" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E72" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1598,18 +1622,18 @@
         <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E73" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1617,13 +1641,13 @@
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1631,13 +1655,13 @@
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E76" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1645,13 +1669,13 @@
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1659,13 +1683,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1673,88 +1697,388 @@
         <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="B83" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>4</v>
+      </c>
+      <c r="E83" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="B84" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="B85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="B87" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="B88" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="B89" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="B90" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" t="s">
+        <v>13</v>
+      </c>
+      <c r="D90" t="s">
+        <v>5</v>
+      </c>
+      <c r="E90" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="B91" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="B93" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="B94" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" t="s">
+        <v>11</v>
+      </c>
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="B95" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="B96" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="E96" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="B97" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="B99" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="B100" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" t="s">
+        <v>5</v>
+      </c>
+      <c r="E100" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="B101" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="B102" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" t="s">
+        <v>13</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:5">
-      <c r="B81" t="s">
-        <v>19</v>
-      </c>
-      <c r="C81" t="s">
-        <v>4</v>
-      </c>
-      <c r="D81" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5">
-      <c r="B82" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" t="s">
-        <v>9</v>
-      </c>
-      <c r="D82" t="s">
-        <v>5</v>
-      </c>
-      <c r="E82" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5">
-      <c r="B83" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" t="s">
-        <v>7</v>
-      </c>
-      <c r="D83" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5">
-      <c r="B84" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s">
-        <v>10</v>
-      </c>
-      <c r="D84" t="s">
-        <v>8</v>
-      </c>
-      <c r="E84" t="s">
+    <row r="105" spans="1:5">
+      <c r="B105" t="s">
+        <v>19</v>
+      </c>
+      <c r="C105" t="s">
+        <v>12</v>
+      </c>
+      <c r="D105" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="B106" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="B107" t="s">
+        <v>19</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="B108" t="s">
+        <v>19</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="B109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" t="s">
+        <v>10</v>
+      </c>
+      <c r="D109" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5">
-      <c r="B85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" t="s">
-        <v>13</v>
-      </c>
-      <c r="D85" t="s">
-        <v>12</v>
-      </c>
-      <c r="E85" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ft && fix: removed not valid cuts && lp gap
</commit_message>
<xml_diff>
--- a/data/campeonato_10_1.xlsx
+++ b/data/campeonato_10_1.xlsx
@@ -77,109 +77,109 @@
     <t>1/1/2022</t>
   </si>
   <si>
+    <t>6:2</t>
+  </si>
+  <si>
+    <t>1:3</t>
+  </si>
+  <si>
     <t>3:0</t>
   </si>
   <si>
+    <t>4:1</t>
+  </si>
+  <si>
+    <t>2:2</t>
+  </si>
+  <si>
+    <t>2:1</t>
+  </si>
+  <si>
+    <t>5:7</t>
+  </si>
+  <si>
+    <t>1:4</t>
+  </si>
+  <si>
+    <t>1:1</t>
+  </si>
+  <si>
+    <t>5:8</t>
+  </si>
+  <si>
+    <t>6:4</t>
+  </si>
+  <si>
+    <t>0:2</t>
+  </si>
+  <si>
+    <t>5:0</t>
+  </si>
+  <si>
+    <t>0:5</t>
+  </si>
+  <si>
+    <t>7:4</t>
+  </si>
+  <si>
+    <t>2:3</t>
+  </si>
+  <si>
+    <t>4:2</t>
+  </si>
+  <si>
+    <t>0:4</t>
+  </si>
+  <si>
+    <t>2:0</t>
+  </si>
+  <si>
+    <t>2:5</t>
+  </si>
+  <si>
     <t>3:4</t>
   </si>
   <si>
+    <t>1:0</t>
+  </si>
+  <si>
+    <t>6:1</t>
+  </si>
+  <si>
+    <t>3:2</t>
+  </si>
+  <si>
+    <t>1:5</t>
+  </si>
+  <si>
+    <t>1:2</t>
+  </si>
+  <si>
+    <t>4:5</t>
+  </si>
+  <si>
+    <t>3:1</t>
+  </si>
+  <si>
+    <t>0:1</t>
+  </si>
+  <si>
+    <t>0:6</t>
+  </si>
+  <si>
+    <t>2:4</t>
+  </si>
+  <si>
+    <t>4:0</t>
+  </si>
+  <si>
+    <t>0:3</t>
+  </si>
+  <si>
+    <t>5:1</t>
+  </si>
+  <si>
     <t>3:3</t>
-  </si>
-  <si>
-    <t>6:0</t>
-  </si>
-  <si>
-    <t>2:5</t>
-  </si>
-  <si>
-    <t>2:3</t>
-  </si>
-  <si>
-    <t>3:2</t>
-  </si>
-  <si>
-    <t>4:2</t>
-  </si>
-  <si>
-    <t>4:0</t>
-  </si>
-  <si>
-    <t>1:2</t>
-  </si>
-  <si>
-    <t>5:4</t>
-  </si>
-  <si>
-    <t>0:2</t>
-  </si>
-  <si>
-    <t>5:0</t>
-  </si>
-  <si>
-    <t>2:4</t>
-  </si>
-  <si>
-    <t>1:5</t>
-  </si>
-  <si>
-    <t>1:1</t>
-  </si>
-  <si>
-    <t>6:2</t>
-  </si>
-  <si>
-    <t>7:3</t>
-  </si>
-  <si>
-    <t>4:3</t>
-  </si>
-  <si>
-    <t>2:2</t>
-  </si>
-  <si>
-    <t>1:4</t>
-  </si>
-  <si>
-    <t>1:3</t>
-  </si>
-  <si>
-    <t>7:1</t>
-  </si>
-  <si>
-    <t>1:6</t>
-  </si>
-  <si>
-    <t>6:4</t>
-  </si>
-  <si>
-    <t>3:5</t>
-  </si>
-  <si>
-    <t>3:1</t>
-  </si>
-  <si>
-    <t>1:0</t>
-  </si>
-  <si>
-    <t>2:1</t>
-  </si>
-  <si>
-    <t>5:5</t>
-  </si>
-  <si>
-    <t>6:3</t>
-  </si>
-  <si>
-    <t>5:2</t>
-  </si>
-  <si>
-    <t>0:4</t>
-  </si>
-  <si>
-    <t>4:1</t>
-  </si>
-  <si>
-    <t>3:6</t>
   </si>
 </sst>
 </file>
@@ -542,10 +542,10 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -562,7 +562,7 @@
         <v>13</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -576,10 +576,10 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -593,7 +593,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -610,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -627,10 +627,10 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -661,10 +661,10 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -678,10 +678,10 @@
         <v>12</v>
       </c>
       <c r="D10">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -695,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="D11">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -741,10 +741,10 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -769,7 +769,7 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -783,10 +783,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -797,10 +797,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
         <v>24</v>
@@ -816,10 +816,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
@@ -830,10 +830,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
         <v>26</v>
@@ -844,10 +844,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
@@ -858,10 +858,10 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -872,13 +872,13 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -891,13 +891,13 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -905,10 +905,10 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
@@ -919,13 +919,13 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -933,13 +933,13 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -947,13 +947,13 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -966,13 +966,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -980,13 +980,13 @@
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -994,13 +994,13 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1008,13 +1008,13 @@
         <v>19</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1022,10 +1022,10 @@
         <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
         <v>35</v>
@@ -1041,13 +1041,13 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1058,10 +1058,10 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1069,13 +1069,13 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1083,13 +1083,13 @@
         <v>19</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1097,13 +1097,13 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1116,13 +1116,13 @@
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1130,13 +1130,13 @@
         <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1144,13 +1144,13 @@
         <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1158,13 +1158,13 @@
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E36" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1175,10 +1175,10 @@
         <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1191,13 +1191,13 @@
         <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1205,13 +1205,13 @@
         <v>19</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
       </c>
       <c r="E40" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1219,13 +1219,13 @@
         <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1233,13 +1233,13 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1247,13 +1247,13 @@
         <v>19</v>
       </c>
       <c r="C43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1266,13 +1266,13 @@
         <v>19</v>
       </c>
       <c r="C45" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1280,13 +1280,13 @@
         <v>19</v>
       </c>
       <c r="C46" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1294,13 +1294,13 @@
         <v>19</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1308,13 +1308,13 @@
         <v>19</v>
       </c>
       <c r="C48" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1325,10 +1325,10 @@
         <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1341,13 +1341,13 @@
         <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1355,13 +1355,13 @@
         <v>19</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1369,13 +1369,13 @@
         <v>19</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1386,10 +1386,10 @@
         <v>13</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E54" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1397,13 +1397,13 @@
         <v>19</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E55" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1416,13 +1416,13 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1430,13 +1430,13 @@
         <v>19</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E58" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1444,13 +1444,13 @@
         <v>19</v>
       </c>
       <c r="C59" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1458,13 +1458,13 @@
         <v>19</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E60" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1472,13 +1472,13 @@
         <v>19</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D61" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1491,13 +1491,13 @@
         <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1505,13 +1505,13 @@
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1519,13 +1519,13 @@
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1533,13 +1533,13 @@
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E66" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1550,10 +1550,10 @@
         <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E67" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1566,10 +1566,10 @@
         <v>19</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E69" t="s">
         <v>46</v>
@@ -1580,13 +1580,13 @@
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E70" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1594,13 +1594,13 @@
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E71" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1608,13 +1608,13 @@
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D72" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E72" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1622,13 +1622,13 @@
         <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E73" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1641,13 +1641,13 @@
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D75" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E75" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1655,13 +1655,13 @@
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1669,13 +1669,13 @@
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D77" t="s">
         <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1683,13 +1683,13 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E78" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1697,10 +1697,10 @@
         <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E79" t="s">
         <v>50</v>
@@ -1719,10 +1719,10 @@
         <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E81" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1733,10 +1733,10 @@
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E82" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1744,13 +1744,13 @@
         <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D83" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E83" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1761,10 +1761,10 @@
         <v>8</v>
       </c>
       <c r="D84" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1772,13 +1772,13 @@
         <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E85" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1791,13 +1791,13 @@
         <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D87" t="s">
         <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1805,13 +1805,13 @@
         <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E88" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1819,13 +1819,13 @@
         <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D89" t="s">
         <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1833,13 +1833,13 @@
         <v>19</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D90" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E90" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1847,13 +1847,13 @@
         <v>19</v>
       </c>
       <c r="C91" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E91" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1866,13 +1866,13 @@
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D93" t="s">
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1883,10 +1883,10 @@
         <v>12</v>
       </c>
       <c r="D94" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E94" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1894,13 +1894,13 @@
         <v>19</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D95" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -1911,7 +1911,7 @@
         <v>6</v>
       </c>
       <c r="D96" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E96" t="s">
         <v>21</v>
@@ -1928,7 +1928,7 @@
         <v>9</v>
       </c>
       <c r="E97" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -1944,10 +1944,10 @@
         <v>4</v>
       </c>
       <c r="D99" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E99" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -1955,13 +1955,13 @@
         <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D100" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E100" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -1969,13 +1969,13 @@
         <v>19</v>
       </c>
       <c r="C101" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D101" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E101" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1983,13 +1983,13 @@
         <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E102" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1997,13 +1997,13 @@
         <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D103" t="s">
         <v>10</v>
       </c>
       <c r="E103" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2016,13 +2016,13 @@
         <v>19</v>
       </c>
       <c r="C105" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2030,13 +2030,13 @@
         <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D106" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2047,10 +2047,10 @@
         <v>8</v>
       </c>
       <c r="D107" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E107" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2058,13 +2058,13 @@
         <v>19</v>
       </c>
       <c r="C108" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E108" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2072,13 +2072,13 @@
         <v>19</v>
       </c>
       <c r="C109" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D109" t="s">
         <v>13</v>
       </c>
       <c r="E109" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>